<commit_message>
update memory map & get e820 info
</commit_message>
<xml_diff>
--- a/doc/MCS Memory Map.xlsx
+++ b/doc/MCS Memory Map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccube\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccube\Desktop\_\os\MCS\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E8E2DF-4CC6-49D3-BAD0-1C3361607EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B664D6C-0D82-41A8-8B43-15D4F5553827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{760B1340-F83B-41FB-B089-5187CF0C4408}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
   <si>
     <t>MCS Memory Map</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -312,6 +312,30 @@
   </si>
   <si>
     <t>0x300000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e820和内核栈保护区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x000f0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x000fffff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x10000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预留内存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROM-BIOS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -775,39 +799,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -817,54 +808,114 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -874,71 +925,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
@@ -946,29 +940,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
@@ -976,8 +961,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,446 +1317,486 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDB2CE3-A67B-4F23-B93E-F53404C1C217}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="15"/>
-    <col min="2" max="2" width="11.109375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="14" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="14"/>
-    <col min="5" max="5" width="11.109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="14"/>
-    <col min="7" max="7" width="11.109375" style="14" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="14"/>
-    <col min="9" max="9" width="11.109375" style="14" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="14"/>
-    <col min="11" max="13" width="11.109375" style="14" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" style="15" customWidth="1"/>
-    <col min="15" max="19" width="8.88671875" style="14"/>
-    <col min="20" max="20" width="11.109375" style="14" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="11.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="11.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="11.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="3"/>
+    <col min="9" max="9" width="11.109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="3"/>
+    <col min="11" max="13" width="11.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="4" customWidth="1"/>
+    <col min="15" max="19" width="8.88671875" style="3"/>
+    <col min="20" max="20" width="11.109375" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="70"/>
     </row>
     <row r="2" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="17" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="17" t="s">
+      <c r="G2" s="64"/>
+      <c r="H2" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="17" t="s">
+      <c r="I2" s="64"/>
+      <c r="J2" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="19"/>
+      <c r="K2" s="64"/>
     </row>
     <row r="3" spans="1:20" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="58" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="36" t="s">
+      <c r="G3" s="49"/>
+      <c r="H3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36" t="s">
+      <c r="I3" s="65"/>
+      <c r="J3" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="15" t="s">
+      <c r="K3" s="66"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="28" t="s">
+      <c r="O3" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
     </row>
     <row r="4" spans="1:20" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="60" t="s">
+      <c r="E4" s="26"/>
+      <c r="F4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="61"/>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="23"/>
+      <c r="H4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="3" t="s">
+      <c r="I4" s="12"/>
+      <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="39"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="60" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="3" t="s">
+      <c r="G5" s="23"/>
+      <c r="H5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="3" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="39"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="60" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="61"/>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="23"/>
+      <c r="H6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="39"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="62" t="s">
+      <c r="E7" s="16"/>
+      <c r="F7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="63"/>
-      <c r="H7" s="44" t="s">
+      <c r="G7" s="21"/>
+      <c r="H7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="45"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="46"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:20" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="64" t="s">
+      <c r="E8" s="29"/>
+      <c r="F8" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="65"/>
-      <c r="H8" s="51" t="s">
+      <c r="G8" s="34"/>
+      <c r="H8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="52"/>
-      <c r="J8" s="51" t="s">
+      <c r="I8" s="31"/>
+      <c r="J8" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="K8" s="53"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:20" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="49" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="64" t="s">
+      <c r="E9" s="29"/>
+      <c r="F9" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="65"/>
-      <c r="H9" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="52"/>
-      <c r="J9" s="51" t="s">
+      <c r="G9" s="34"/>
+      <c r="H9" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="31"/>
+      <c r="J9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="53"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:20" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="36"/>
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="66" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="26" t="s">
+      <c r="G10" s="47"/>
+      <c r="H10" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
     </row>
     <row r="11" spans="1:20" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="58" t="s">
+      <c r="E11" s="42"/>
+      <c r="F11" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="59"/>
-      <c r="H11" s="34" t="s">
+      <c r="G11" s="49"/>
+      <c r="H11" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="34" t="s">
+      <c r="I11" s="44"/>
+      <c r="J11" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="54"/>
+      <c r="K11" s="45"/>
     </row>
     <row r="12" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="62" t="s">
+      <c r="E12" s="16"/>
+      <c r="F12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="63"/>
-      <c r="H12" s="44" t="s">
+      <c r="G12" s="21"/>
+      <c r="H12" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="45"/>
-      <c r="J12" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="46"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:20" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="68" t="s">
+      <c r="E13" s="52"/>
+      <c r="F13" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="69"/>
-      <c r="H13" s="20" t="s">
+      <c r="G13" s="56"/>
+      <c r="H13" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="54"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="60" t="s">
+      <c r="E14" s="26"/>
+      <c r="F14" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="61"/>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="23"/>
+      <c r="H14" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="3" t="s">
+      <c r="I14" s="12"/>
+      <c r="J14" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="K14" s="4"/>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="24" t="s">
+      <c r="A15" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="59"/>
+      <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="57"/>
-      <c r="F15" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="61"/>
-      <c r="H15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K15" s="4"/>
+      <c r="D15" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="60"/>
+      <c r="F15" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="1" t="s">
+      <c r="A16" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="59"/>
+      <c r="C16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="61"/>
-      <c r="H16" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K16" s="4"/>
+      <c r="D16" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="60"/>
+      <c r="F16" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="23"/>
+      <c r="H16" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="23"/>
+      <c r="H17" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="2" t="s">
+      <c r="B18" s="51"/>
+      <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="60" t="s">
+      <c r="E18" s="26"/>
+      <c r="F18" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="61"/>
-      <c r="H17" s="3" t="s">
+      <c r="G18" s="23"/>
+      <c r="H18" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="4"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="81">
+  <mergeCells count="86">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="O3:T3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -1754,16 +1818,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="H14:I14"/>

</xml_diff>